<commit_message>
first_name and last_name feild added in upload sales agent
</commit_message>
<xml_diff>
--- a/public/assests/Sample_Sales_Agent.xlsx
+++ b/public/assests/Sample_Sales_Agent.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Sr. No.</t>
   </si>
   <si>
-    <t>User Name</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
   <si>
     <t>Contact No.</t>
@@ -73,16 +76,22 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>+914567893210</t>
+  </si>
+  <si>
+    <t>testuser@yopmail.com</t>
+  </si>
+  <si>
+    <t>rndx92jf8a</t>
+  </si>
+  <si>
     <t>Test User</t>
-  </si>
-  <si>
-    <t>+914567893210</t>
-  </si>
-  <si>
-    <t>testuser@yopmail.com</t>
-  </si>
-  <si>
-    <t>rndx92jf8a</t>
   </si>
   <si>
     <t>876543219012</t>
@@ -114,7 +123,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,15 +363,18 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="7" width="11.22"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -414,8 +425,11 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -423,61 +437,64 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1">
         <v>10.0</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="1">
         <v>0.0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="1">
         <v>0.0</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="1">
         <v>0.0</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="1">
         <v>0.0</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="1">
         <v>0.0</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="1">
         <v>1.0</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>2.0</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>